<commit_message>
Create dishes database and mod ingr database
</commit_message>
<xml_diff>
--- a/Demo/sample.xlsx
+++ b/Demo/sample.xlsx
@@ -14,12 +14,7 @@
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -38,6 +33,9 @@
     <t>Чел 1</t>
   </si>
   <si>
+    <t>чел 2</t>
+  </si>
+  <si>
     <t>Чел 3</t>
   </si>
   <si>
@@ -57,9 +55,6 @@
   </si>
   <si>
     <t>Чел 9</t>
-  </si>
-  <si>
-    <t>чел 2</t>
   </si>
 </sst>
 </file>
@@ -381,7 +376,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C10"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,7 +408,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>2000</v>
@@ -424,7 +419,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>3000</v>
@@ -435,7 +430,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>4000</v>
@@ -446,7 +441,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <v>5000</v>
@@ -457,7 +452,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C7">
         <v>6000</v>
@@ -468,7 +463,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C8">
         <v>7000</v>
@@ -479,7 +474,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C9">
         <v>8000</v>
@@ -490,7 +485,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C10">
         <v>9000</v>

</xml_diff>